<commit_message>
Add new localized file names and update binary files
- Added a new localized file name for the image "�ù��^���e�� 2025-11-01 134041.png" in desktop.ini.
- Updated the binary file "繪圖用.xlsx" with new content.
- Added a new binary file "Supporter 比例圖_Eng.png" with image data.
- Updated the existing binary file "繪圖用.xlsx" with new content.
</commit_message>
<xml_diff>
--- a/data/繪圖用.xlsx
+++ b/data/繪圖用.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\projects\osu_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4808EA-5B88-4154-9A28-5EBCB7972216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C443E88-3FDD-431D-8ECB-81F79F41D32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{921BFFB4-7898-4B54-8CB7-17A9B4476068}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{921BFFB4-7898-4B54-8CB7-17A9B4476068}"/>
   </bookViews>
   <sheets>
     <sheet name="Supporter 與留存關係" sheetId="1" r:id="rId1"/>
@@ -310,62 +310,8 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
-                    <a:ea typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="zh-TW"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
+            <c:extLst/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -405,6 +351,287 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9435-4492-9E35-9719B5EDA359}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1542981711"/>
+        <c:axId val="1542980047"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1542981711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
+                <a:ea typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1542980047"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1542980047"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1542981711"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
+          <a:ea typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
+                <a:ea typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW"/>
+              <a:t>Proportion of Supporters </a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="1.9444444444444445E-2"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
+              <a:ea typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Supporter 與留存關係'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>贊助者比例</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Supporter 與留存關係'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>early_churn_users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>trial_users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>retained_users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Supporter 與留存關係'!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.9999999999999995E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5999999999999999E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-31B3-4390-9A58-030A7ED417E5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -579,7 +806,550 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1115,6 +1885,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>676604</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>52552</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>937861</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>36222</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="圖表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A345EF4-FB9F-4783-BC4A-FDC23AAE2D59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1169,6 +1977,60 @@
               <a:ea typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
             </a:rPr>
             <a:t>各贊助者佔該分群的比例</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.00761</cdr:x>
+      <cdr:y>0.10996</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.26881</cdr:x>
+      <cdr:y>0.18009</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="文字方塊 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0249E8F-27FB-4F1C-8BFF-53AE5BD3BE87}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="34816" y="298701"/>
+          <a:ext cx="1195552" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="700">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
+              <a:ea typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
+            </a:rPr>
+            <a:t>Proportion of Supporters within each segment</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -1476,8 +2338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535FED29-B06C-49AD-8CAF-1FFF75B0FA26}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1622,7 +2484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F56E42A-A665-4E09-AE03-398949A155CB}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>